<commit_message>
Disable most of level 1; convert platforms into pymunk objects
</commit_message>
<xml_diff>
--- a/scripts/leveldesigner/level_data.xlsx
+++ b/scripts/leveldesigner/level_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidellis/PycharmProjects/tCS-Platformer/scripts/leveldesigner/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikhil\PycharmProjects\tCS-Platformer\scripts\leveldesigner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8201AF95-6373-374A-A568-8250155D9796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A8A121-F4B1-4B18-B110-EC9D851529B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340"/>
+    <workbookView xWindow="-20355" yWindow="2295" windowWidth="19425" windowHeight="15435" tabRatio="488" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="level1_data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -562,33 +562,11 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAF7533"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAF7533"/>
         </patternFill>
       </fill>
     </dxf>
@@ -603,66 +581,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightGrid">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightGrid">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightGrid">
-          <fgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightGrid">
-          <fgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor rgb="FFAF7533"/>
         </patternFill>
       </fill>
     </dxf>
@@ -980,16 +899,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BZ20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="3" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1225,7 +1142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1461,7 +1378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1697,7 +1614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1933,7 +1850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2169,7 +2086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -2405,7 +2322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -2641,7 +2558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -2877,7 +2794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -3113,7 +3030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -3349,7 +3266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -3585,7 +3502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -3821,7 +3738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -4057,7 +3974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -4293,7 +4210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -4529,7 +4446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -4765,7 +4682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -5001,7 +4918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -5237,7 +5154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -5473,7 +5390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:78" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -5711,13 +5628,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:BZ20">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="a">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="a">
       <formula>NOT(ISERROR(SEARCH("a",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="z">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="z">
       <formula>NOT(ISERROR(SEARCH("z",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add portal object to advance from level to level
</commit_message>
<xml_diff>
--- a/scripts/leveldesigner/level_data.xlsx
+++ b/scripts/leveldesigner/level_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikhil\PycharmProjects\tCS-Platformer\scripts\leveldesigner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99198F4-10F1-4DD7-87C3-81D856AE987C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0259A683-9E14-4D76-8861-66E46AC96B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20670" yWindow="-7830" windowWidth="19425" windowHeight="14250" tabRatio="488" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="5">
   <si>
     <t>a</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>e</t>
+  </si>
+  <si>
+    <t>p</t>
   </si>
 </sst>
 </file>
@@ -565,26 +568,11 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAF7533"/>
+          <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -934,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BZ20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BX9" sqref="BX9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2583,7 +2571,7 @@
         <v>1</v>
       </c>
       <c r="BX7" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="BY7" s="1" t="s">
         <v>1</v>
@@ -3282,13 +3270,13 @@
         <v>1</v>
       </c>
       <c r="BU10" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BV10" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BW10" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BX10" s="1" t="s">
         <v>1</v>
@@ -3978,13 +3966,13 @@
         <v>1</v>
       </c>
       <c r="BQ13" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BR13" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BS13" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BT13" s="1" t="s">
         <v>1</v>
@@ -4671,13 +4659,13 @@
         <v>1</v>
       </c>
       <c r="BL16" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BM16" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BN16" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BO16" s="1" t="s">
         <v>1</v>
@@ -5662,17 +5650,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:BZ20">
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="a">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="a">
       <formula>NOT(ISERROR(SEARCH("a",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="z">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="z">
       <formula>NOT(ISERROR(SEARCH("z",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="e">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="e">
       <formula>NOT(ISERROR(SEARCH("e",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="p">
+      <formula>NOT(ISERROR(SEARCH("p",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>